<commit_message>
Commit made to excel file
</commit_message>
<xml_diff>
--- a/SpreadSheet2020/data.xlsx
+++ b/SpreadSheet2020/data.xlsx
@@ -31,46 +31,46 @@
     <t>Max Sales</t>
   </si>
   <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
     <t>Total Sales</t>
   </si>
   <si>
     <t>Average Sales</t>
-  </si>
-  <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Feb</t>
-  </si>
-  <si>
-    <t>March</t>
-  </si>
-  <si>
-    <t>April</t>
-  </si>
-  <si>
-    <t>May</t>
-  </si>
-  <si>
-    <t>June</t>
-  </si>
-  <si>
-    <t>July</t>
-  </si>
-  <si>
-    <t>August</t>
-  </si>
-  <si>
-    <t>September</t>
-  </si>
-  <si>
-    <t>October</t>
-  </si>
-  <si>
-    <t>Nov</t>
-  </si>
-  <si>
-    <t>Dec</t>
   </si>
 </sst>
 </file>
@@ -402,13 +402,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -419,85 +419,89 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>